<commit_message>
updated known issues tab
</commit_message>
<xml_diff>
--- a/ActivityModifier/ActivityModifier_dev_log.xlsx
+++ b/ActivityModifier/ActivityModifier_dev_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Qingshi/Documents/RecurDig/ActivityModifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777455F5-6ABA-CE4E-B261-556A1C20053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D46500-BC23-2447-9B19-4452F64B47CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="4" xr2:uid="{EC2A7457-63DE-4444-B7E6-13A8F69C74F8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>Current ver</t>
   </si>
@@ -678,6 +678,18 @@
   </si>
   <si>
     <t>https://docs.google.com/document/d/1gI1pTNg77BfHOhjcY9HtXS7_aJfSspwzJBG89WlRZr8/edit#</t>
+  </si>
+  <si>
+    <t>need to enforce unit conversion between parent and child layers (and log each instance of unit conversion)</t>
+  </si>
+  <si>
+    <t>Currently unit difference is not checked between parent and child layers (e.g., parent layer uses 'MJ' for electricity input, but electricity generation (child layer) is in the unit of 'kWh')</t>
+  </si>
+  <si>
+    <t>The amount of child layer activity may not be correct (as current code multiplies the amt of parent activity with the amt of child activity, without considering the difference in units)</t>
+  </si>
+  <si>
+    <t>ß</t>
   </si>
 </sst>
 </file>
@@ -1472,10 +1484,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0230F2A-7B4C-BB44-9DFE-BFCCE1DC2F69}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1486,7 +1498,7 @@
     <col min="4" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17">
+    <row r="1" spans="1:10" ht="17">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1500,7 +1512,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17">
+    <row r="2" spans="1:10" ht="17">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -1514,7 +1526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="34">
+    <row r="3" spans="1:10" ht="34">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -1525,7 +1537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="34">
+    <row r="4" spans="1:10" ht="34">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -1533,7 +1545,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="34">
+    <row r="5" spans="1:10" ht="34">
       <c r="A5" s="8" t="s">
         <v>59</v>
       </c>
@@ -1541,7 +1553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="34">
+    <row r="6" spans="1:10" ht="34">
       <c r="A6" s="8" t="s">
         <v>61</v>
       </c>
@@ -1550,6 +1562,22 @@
       </c>
       <c r="C6" s="8" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="68">
+      <c r="A7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="J12" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>